<commit_message>
Can now find all groupings of users from assign button
</commit_message>
<xml_diff>
--- a/ExcelPropertyManagement.xlsx
+++ b/ExcelPropertyManagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacco\School\SER416\FinalProject\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D6C801-0275-44D1-B90B-D34F8DA5AE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E0B6F2-711C-4231-9041-91E2DABE3D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="900" windowWidth="16110" windowHeight="15300" tabRatio="911" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="0" windowWidth="16110" windowHeight="15300" tabRatio="911" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="18" r:id="rId1"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="143">
   <si>
     <t>Date</t>
   </si>
@@ -782,15 +782,6 @@
   <si>
     <t>Payment Recieved</t>
   </si>
-  <si>
-    <t>NIck Angel</t>
-  </si>
-  <si>
-    <t>MOVE OUT 4/15/2022</t>
-  </si>
-  <si>
-    <t>Rent: 4 ' 2022</t>
-  </si>
 </sst>
 </file>
 
@@ -981,7 +972,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1053,12 +1044,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1218,7 +1203,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1363,10 +1348,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2007,10 +1988,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914380C8-C1D0-4A60-82DC-17615EEB8410}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2084,23 +2065,24 @@
       </c>
       <c r="K3" s="87" t="str" cm="1">
         <f t="array" ref="K3">LOOKUP(2,1/(J:J&lt;&gt;""),J:J)</f>
-        <v>NIck Angel</v>
+        <v>Alex Zacco</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15">
       <c r="A4">
-        <f>COUNTIF(A6:A65539, "&lt;&gt;")</f>
-        <v>2</v>
+        <f>COUNTIF(A6:A65537, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="D4" s="51">
-        <f>INDEX(D6:D65538, A4)</f>
-        <v>0</v>
+        <f>INDEX(D6:D65536, A4)</f>
+        <v>44620</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="50" t="s">
         <v>78</v>
       </c>
       <c r="H4" s="50">
+        <f>INDEX(H6:H65538, A4)</f>
         <v>2500</v>
       </c>
       <c r="I4" s="53">
@@ -2169,90 +2151,68 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="98" customFormat="1">
-      <c r="A7" s="99"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="99" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99" t="s">
-        <v>113</v>
-      </c>
+    <row r="7" spans="1:11" s="65" customFormat="1">
+      <c r="A7" s="98"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
     </row>
     <row r="8" spans="1:11" s="65" customFormat="1">
-      <c r="A8" s="102">
-        <v>4</v>
-      </c>
-      <c r="B8" s="102">
-        <v>2022</v>
-      </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="103">
-        <v>44666</v>
-      </c>
-      <c r="E8" s="102" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="104">
-        <v>1000</v>
-      </c>
-      <c r="G8" s="104">
-        <v>3500</v>
-      </c>
-      <c r="H8" s="104">
-        <v>2500</v>
-      </c>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102" t="s">
-        <v>143</v>
-      </c>
+      <c r="A8" s="98"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
     </row>
     <row r="9" spans="1:11" s="65" customFormat="1">
-      <c r="A9" s="102"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-    </row>
-    <row r="10" spans="1:11" s="65" customFormat="1">
-      <c r="A10" s="102"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-    </row>
-    <row r="11" spans="1:11" s="65" customFormat="1">
+      <c r="D9" s="97"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+    </row>
+    <row r="10" spans="1:11" ht="15">
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="96"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="97"/>
+      <c r="E11" s="65"/>
       <c r="F11" s="64"/>
       <c r="G11" s="64"/>
       <c r="H11" s="64"/>
-    </row>
-    <row r="12" spans="1:11" ht="15">
+      <c r="I11" s="65"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="65"/>
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
       <c r="D12" s="97"/>
       <c r="E12" s="65"/>
-      <c r="F12" s="95"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="64"/>
       <c r="H12" s="64"/>
-      <c r="I12" s="96"/>
+      <c r="I12" s="65"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="65"/>
@@ -2275,28 +2235,6 @@
       <c r="G14" s="64"/>
       <c r="H14" s="64"/>
       <c r="I14" s="65"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="65"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2309,11 +2247,11 @@
   <dimension ref="A1:M298"/>
   <sheetViews>
     <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D227" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D212" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2:H3"/>
       <selection pane="topRight" activeCell="H2" sqref="H2:H3"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2:H3"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2:K3"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2404,6 +2342,7 @@
         <v>78</v>
       </c>
       <c r="H4" s="50">
+        <f>INDEX(H6:H65538, A4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="53">
@@ -10678,7 +10617,7 @@
       <selection activeCell="F254" sqref="F254"/>
       <selection pane="topRight" activeCell="F254" sqref="F254"/>
       <selection pane="bottomLeft" activeCell="F254" sqref="F254"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16246,7 +16185,7 @@
       <selection activeCell="F254" sqref="F254"/>
       <selection pane="topRight" activeCell="F254" sqref="F254"/>
       <selection pane="bottomLeft" activeCell="F254" sqref="F254"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3:K4"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22593,7 +22532,7 @@
       <selection activeCell="F254" sqref="F254"/>
       <selection pane="topRight" activeCell="F254" sqref="F254"/>
       <selection pane="bottomLeft" activeCell="F254" sqref="F254"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>